<commit_message>
Revert "up to 04b528"
This reverts commit c8b7782f370ad1efb8bb7285e154653f998e4120.
</commit_message>
<xml_diff>
--- a/doc/help_dialogs/Input_files/keyboardshortcuts.xlsx
+++ b/doc/help_dialogs/Input_files/keyboardshortcuts.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Keyboard Shortcuts" sheetId="1" state="visible" r:id="rId2"/>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="260" uniqueCount="208">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="238" uniqueCount="190">
   <si>
     <t xml:space="preserve">KEYBOARD SHORTCUTS</t>
   </si>
@@ -37,58 +37,6 @@
   </si>
   <si>
     <t xml:space="preserve">Turns ON/OFF Keyboard Shortcuts</t>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <i val="true"/>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">⌘-</t>
-    </r>
-    <r>
-      <rPr>
-        <i val="true"/>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">ENTER [Mac]\nCTRL+ENTER [Win]</t>
-    </r>
-  </si>
-  <si>
-    <t xml:space="preserve">Starts recording</t>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <i val="true"/>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">SHIFT-</t>
-    </r>
-    <r>
-      <rPr>
-        <i val="true"/>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">ENTER</t>
-    </r>
-  </si>
-  <si>
-    <t xml:space="preserve">Turns Artisan OFF</t>
   </si>
   <si>
     <t xml:space="preserve">SPACE</t>
@@ -98,16 +46,10 @@
 When Keyboard Shortcuts are OFF adds a custom event</t>
   </si>
   <si>
-    <t xml:space="preserve">LEFT,RIGHT</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Change roast event key focus</t>
-  </si>
-  <si>
     <t xml:space="preserve">LEFT,RIGHT,UP,DOWN</t>
   </si>
   <si>
-    <t xml:space="preserve">Move background (when sliders not visible or when Config&gt;&gt; Events&gt;&gt; Sliders tab&gt;&gt; Keyboard Control is not selected)</t>
+    <t xml:space="preserve">Move background or key focus</t>
   </si>
   <si>
     <t xml:space="preserve">A</t>
@@ -260,7 +202,7 @@
     <t xml:space="preserve">Q,W,E,R + &lt;value&gt;</t>
   </si>
   <si>
-    <t xml:space="preserve">Quick Special Event Entry.  The keys q,w,e, and r correspond to special events 1,2,3 and 4.  A two digit numeric value must follow the shortcut letter, e.g. 'q75', when the correspoding event slider max value is 100 or less (default setting).   When the slider max value is greater than 100, three digits must be entered and for values less than 100 a leading zero is required, e.g. 'q075'.  </t>
+    <t xml:space="preserve">Quick Special Event Entry.  The keys q,w,e, and r correspond to special events 1,2,3 and 4.  A two digit numeric value must follow the shortcut letter, e.g. 'q75', when the correspoding event slider max value is 100 or less (default setting).   When the slider max value is greater than 100, three digits must be entered and for values less that 100 a leading zero is required, e.g. 'q075'.  </t>
   </si>
   <si>
     <t xml:space="preserve">V +  &lt;value&gt;</t>
@@ -308,10 +250,7 @@
     <t xml:space="preserve">Requires an artisan.plus account</t>
   </si>
   <si>
-    <t xml:space="preserve">Double Click on Background Profile Title</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Graph &amp; Designer</t>
+    <t xml:space="preserve">Click on Background Profile Title</t>
   </si>
   <si>
     <t xml:space="preserve">Toggle Show/Hide Background Profile</t>
@@ -371,6 +310,33 @@
     <t xml:space="preserve">Toggle debug logging mode</t>
   </si>
   <si>
+    <t xml:space="preserve">Click on timer</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Simulator</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Toggle Pause/Continue Simulation</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Simulator speed may be changd while paused.  See next two shortcuts.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">OPTION Tools&gt;&gt;Simulator [Mac]\nALT Tools&gt;&gt;Simulator [Win]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Graph/Simulator</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Start or change Simulator speed to 2x mode</t>
+  </si>
+  <si>
+    <t xml:space="preserve">⌘ Tools&gt;&gt;Simulator [Mac]\nCTRL Tools&gt;&gt;Simulator [Win]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Start or change Simulator speed to 4x mode</t>
+  </si>
+  <si>
     <t xml:space="preserve">Click on LCD</t>
   </si>
   <si>
@@ -411,68 +377,6 @@
   </si>
   <si>
     <t xml:space="preserve">Device = &lt;all others&gt;, Control enabled in Config&gt;&gt; Device</t>
-  </si>
-  <si>
-    <t xml:space="preserve">TAB</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Graph when Sliders visible</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Sequence slider select</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Requires Keyboard Control enabled in Config&gt;&gt; Events
-Keyboard Shortcuts must be turned off (ENTER)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">UP,DOWN,RIGHT,LEFT</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Increment selected slider up or down by step amount</t>
-  </si>
-  <si>
-    <t xml:space="preserve">OPTION+UP, OPTION+DOWN [Mac]\nPAGEUP,PAGEDOWN [Win]</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Increment selected slider up or down by 10</t>
-  </si>
-  <si>
-    <t xml:space="preserve">HOME,END</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Set selected slider to minimum or maximum value</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Requires Keyboard Control enabled in Config&gt;&gt; Events
-Keyboard Shortcuts must be disabled (ENTER)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">OPTION Tools&gt;&gt;Simulator [Mac]\nALT Tools&gt;&gt;Simulator [Win]</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Graph/Simulator</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Start or change Simulator speed to 2x mode</t>
-  </si>
-  <si>
-    <t xml:space="preserve">⌘ Tools&gt;&gt;Simulator [Mac]\nCTRL Tools&gt;&gt;Simulator [Win]</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Start or change Simulator speed to 4x mode</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Click on timer</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Simulator</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Toggle Pause/Continue Simulation</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Simulator speed may be changd while paused.  See next two shortcuts.</t>
   </si>
   <si>
     <t xml:space="preserve">⌘+C [Mac]\nCTRL+C [Win]</t>
@@ -698,7 +602,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="General"/>
   </numFmts>
-  <fonts count="8">
+  <fonts count="7">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -728,13 +632,6 @@
       <name val="Calibri"/>
       <family val="2"/>
       <charset val="1"/>
-    </font>
-    <font>
-      <i val="true"/>
-      <sz val="11"/>
-      <color rgb="FF000000"/>
-      <name val="Calibri"/>
-      <family val="2"/>
     </font>
     <font>
       <sz val="11"/>
@@ -796,7 +693,7 @@
       <protection locked="true" hidden="false"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="10">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -805,16 +702,12 @@
       <alignment horizontal="general" vertical="top" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
     <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="top" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
@@ -825,6 +718,10 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="20" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -833,15 +730,7 @@
       <alignment horizontal="general" vertical="top" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="20" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -863,10 +752,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:B37"/>
+  <dimension ref="A1:B34"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B5" activeCellId="0" sqref="B5"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A6" activeCellId="0" sqref="A3:A21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.578125" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -888,284 +777,260 @@
         <v>2</v>
       </c>
     </row>
-    <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="2" t="s">
+    <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="1" t="s">
         <v>3</v>
       </c>
       <c r="B3" s="1" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="4" customFormat="false" ht="14.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="3" t="s">
+    <row r="4" customFormat="false" ht="60" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="B4" s="1" t="s">
+      <c r="B4" s="2" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="5" customFormat="false" ht="14.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="3" t="s">
+    <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="1" t="s">
         <v>7</v>
       </c>
       <c r="B5" s="1" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="6" customFormat="false" ht="41.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="2" t="s">
+    <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="B6" s="4" t="s">
+      <c r="B6" s="1" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="7" customFormat="false" ht="14.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="2" t="s">
+    <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="B7" s="4" t="s">
+      <c r="B7" s="1" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="2" t="s">
+      <c r="A8" s="3" t="s">
         <v>13</v>
       </c>
       <c r="B8" s="1" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="2" t="s">
+    <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A9" s="3" t="s">
         <v>15</v>
       </c>
       <c r="B9" s="1" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="10" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="2" t="s">
+    <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A10" s="3" t="s">
         <v>17</v>
       </c>
       <c r="B10" s="1" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="11" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="2" t="s">
+    <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A11" s="3" t="s">
         <v>19</v>
       </c>
       <c r="B11" s="1" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="12" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A12" s="2" t="s">
+    <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A12" s="3" t="s">
         <v>21</v>
       </c>
       <c r="B12" s="1" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="13" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A13" s="2" t="s">
+    <row r="13" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A13" s="3" t="s">
         <v>23</v>
       </c>
       <c r="B13" s="1" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="14" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A14" s="2" t="s">
+    <row r="14" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A14" s="3" t="s">
         <v>25</v>
       </c>
       <c r="B14" s="1" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="15" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A15" s="2" t="s">
+    <row r="15" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A15" s="3" t="s">
         <v>27</v>
       </c>
       <c r="B15" s="1" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="16" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A16" s="2" t="s">
+    <row r="16" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A16" s="3" t="s">
         <v>29</v>
       </c>
       <c r="B16" s="1" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="17" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A17" s="2" t="s">
+    <row r="17" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A17" s="3" t="s">
         <v>31</v>
       </c>
       <c r="B17" s="1" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="18" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A18" s="2" t="s">
+    <row r="18" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A18" s="3" t="s">
         <v>33</v>
       </c>
       <c r="B18" s="1" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="19" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A19" s="2" t="s">
+    <row r="19" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A19" s="3" t="s">
         <v>35</v>
       </c>
       <c r="B19" s="1" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="20" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A20" s="2" t="s">
+    <row r="20" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A20" s="3" t="s">
         <v>37</v>
       </c>
       <c r="B20" s="1" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="21" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A21" s="2" t="s">
+    <row r="21" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A21" s="3" t="s">
         <v>39</v>
       </c>
       <c r="B21" s="1" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="22" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A22" s="2" t="s">
+    <row r="22" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A22" s="3" t="s">
         <v>41</v>
       </c>
       <c r="B22" s="1" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="23" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A23" s="2" t="s">
+    <row r="23" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A23" s="3" t="s">
         <v>43</v>
       </c>
       <c r="B23" s="1" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="24" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A24" s="2" t="s">
+    <row r="24" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A24" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="B24" s="4" t="s">
         <v>45</v>
       </c>
-      <c r="B24" s="1" t="s">
+    </row>
+    <row r="25" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A25" s="3" t="s">
         <v>46</v>
       </c>
-    </row>
-    <row r="25" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A25" s="2" t="s">
+      <c r="B25" s="1" t="s">
         <v>47</v>
       </c>
-      <c r="B25" s="1" t="s">
+    </row>
+    <row r="26" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A26" s="3" t="s">
         <v>48</v>
       </c>
-    </row>
-    <row r="26" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A26" s="2" t="s">
+      <c r="B26" s="1" t="s">
         <v>49</v>
       </c>
-      <c r="B26" s="1" t="s">
+    </row>
+    <row r="27" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A27" s="3" t="s">
         <v>50</v>
       </c>
-    </row>
-    <row r="27" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A27" s="2" t="s">
-        <v>47</v>
-      </c>
-      <c r="B27" s="5" t="s">
+      <c r="B27" s="1" t="s">
         <v>51</v>
       </c>
     </row>
-    <row r="28" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A28" s="2" t="s">
+    <row r="28" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A28" s="3" t="s">
         <v>52</v>
       </c>
       <c r="B28" s="1" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="29" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A29" s="2" t="s">
+    <row r="29" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A29" s="3" t="s">
         <v>54</v>
       </c>
       <c r="B29" s="1" t="s">
         <v>55</v>
       </c>
     </row>
-    <row r="30" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A30" s="2" t="s">
+    <row r="30" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A30" s="3" t="s">
         <v>56</v>
       </c>
       <c r="B30" s="1" t="s">
         <v>57</v>
       </c>
     </row>
-    <row r="31" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A31" s="2" t="s">
+    <row r="31" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A31" s="3" t="s">
         <v>58</v>
       </c>
       <c r="B31" s="1" t="s">
         <v>59</v>
       </c>
     </row>
-    <row r="32" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A32" s="2" t="s">
+    <row r="32" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A32" s="3" t="s">
         <v>60</v>
       </c>
       <c r="B32" s="1" t="s">
         <v>61</v>
       </c>
     </row>
-    <row r="33" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A33" s="2" t="s">
+    <row r="33" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A33" s="3" t="s">
         <v>62</v>
       </c>
       <c r="B33" s="1" t="s">
         <v>63</v>
       </c>
     </row>
-    <row r="34" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A34" s="2" t="s">
+    <row r="34" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A34" s="3" t="s">
         <v>64</v>
       </c>
       <c r="B34" s="1" t="s">
         <v>65</v>
-      </c>
-    </row>
-    <row r="35" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A35" s="2" t="s">
-        <v>66</v>
-      </c>
-      <c r="B35" s="1" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="36" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A36" s="2" t="s">
-        <v>68</v>
-      </c>
-      <c r="B36" s="1" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="37" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A37" s="2" t="s">
-        <v>70</v>
-      </c>
-      <c r="B37" s="1" t="s">
-        <v>71</v>
       </c>
     </row>
   </sheetData>
@@ -1184,469 +1049,413 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:D36"/>
+  <dimension ref="A1:D32"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A21" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A36" activeCellId="0" sqref="A36"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="D32" activeCellId="1" sqref="A3:A21 D32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.15625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="6" width="53"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="6" width="31.43"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="6" width="72.01"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="6" width="45.42"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1024" min="5" style="6" width="9.14"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="5" width="53"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="5" width="31.43"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="5" width="72.01"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="5" width="45.42"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1024" min="5" style="5" width="9.14"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="7" t="s">
+      <c r="A1" s="5" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="5" t="s">
+        <v>67</v>
+      </c>
+      <c r="B2" s="5" t="s">
+        <v>68</v>
+      </c>
+      <c r="C2" s="5" t="s">
+        <v>69</v>
+      </c>
+      <c r="D2" s="5" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="6" t="s">
+        <v>71</v>
+      </c>
+      <c r="B3" s="5" t="s">
         <v>72</v>
       </c>
-    </row>
-    <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="6" t="s">
+      <c r="C3" s="5" t="s">
         <v>73</v>
       </c>
-      <c r="B2" s="6" t="s">
+      <c r="D3" s="5" t="s">
         <v>74</v>
       </c>
-      <c r="C2" s="6" t="s">
+    </row>
+    <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="6" t="s">
         <v>75</v>
       </c>
-      <c r="D2" s="6" t="s">
+      <c r="B4" s="5" t="s">
+        <v>72</v>
+      </c>
+      <c r="C4" s="5" t="s">
         <v>76</v>
       </c>
-    </row>
-    <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="8" t="s">
+      <c r="D4" s="5" t="s">
         <v>77</v>
       </c>
-      <c r="B3" s="6" t="s">
+    </row>
+    <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="6" t="s">
         <v>78</v>
       </c>
-      <c r="C3" s="6" t="s">
+      <c r="B5" s="5" t="s">
+        <v>72</v>
+      </c>
+      <c r="C5" s="5" t="s">
         <v>79</v>
       </c>
-      <c r="D3" s="6" t="s">
+    </row>
+    <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="6" t="s">
         <v>80</v>
       </c>
-    </row>
-    <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="8" t="s">
+      <c r="B6" s="5" t="s">
+        <v>72</v>
+      </c>
+      <c r="C6" s="5" t="s">
         <v>81</v>
       </c>
-      <c r="B4" s="7" t="s">
+    </row>
+    <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="6" t="s">
         <v>82</v>
       </c>
-      <c r="C4" s="6" t="s">
+      <c r="B7" s="5" t="s">
+        <v>72</v>
+      </c>
+      <c r="C7" s="5" t="s">
         <v>83</v>
       </c>
-      <c r="D4" s="6" t="s">
+      <c r="D7" s="5" t="s">
         <v>84</v>
       </c>
     </row>
-    <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="8" t="s">
+    <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A8" s="6" t="s">
         <v>85</v>
       </c>
-      <c r="B5" s="6" t="s">
-        <v>78</v>
-      </c>
-      <c r="C5" s="6" t="s">
+      <c r="B8" s="5" t="s">
+        <v>72</v>
+      </c>
+      <c r="C8" s="5" t="s">
         <v>86</v>
       </c>
     </row>
-    <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="8" t="s">
+    <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A9" s="6" t="s">
         <v>87</v>
       </c>
-      <c r="B6" s="6" t="s">
-        <v>78</v>
-      </c>
-      <c r="C6" s="6" t="s">
+      <c r="B9" s="5" t="s">
+        <v>72</v>
+      </c>
+      <c r="C9" s="5" t="s">
         <v>88</v>
       </c>
     </row>
-    <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="8" t="s">
+    <row r="10" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A10" s="6" t="s">
         <v>89</v>
       </c>
-      <c r="B7" s="6" t="s">
-        <v>78</v>
-      </c>
-      <c r="C7" s="6" t="s">
+      <c r="B10" s="5" t="s">
+        <v>72</v>
+      </c>
+      <c r="C10" s="5" t="s">
         <v>90</v>
       </c>
-      <c r="D7" s="6" t="s">
+    </row>
+    <row r="11" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A11" s="6" t="s">
         <v>91</v>
       </c>
-    </row>
-    <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="8" t="s">
+      <c r="B11" s="5" t="s">
+        <v>72</v>
+      </c>
+      <c r="C11" s="5" t="s">
         <v>92</v>
       </c>
-      <c r="B8" s="6" t="s">
-        <v>78</v>
-      </c>
-      <c r="C8" s="6" t="s">
+    </row>
+    <row r="12" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A12" s="6" t="s">
         <v>93</v>
       </c>
-    </row>
-    <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="8" t="s">
+      <c r="B12" s="5" t="s">
+        <v>72</v>
+      </c>
+      <c r="C12" s="5" t="s">
         <v>94</v>
       </c>
-      <c r="B9" s="6" t="s">
-        <v>78</v>
-      </c>
-      <c r="C9" s="6" t="s">
+    </row>
+    <row r="13" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A13" s="6" t="s">
         <v>95</v>
       </c>
-    </row>
-    <row r="10" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="8" t="s">
+      <c r="B13" s="5" t="s">
         <v>96</v>
       </c>
-      <c r="B10" s="6" t="s">
-        <v>78</v>
-      </c>
-      <c r="C10" s="6" t="s">
+      <c r="C13" s="5" t="s">
         <v>97</v>
       </c>
-    </row>
-    <row r="11" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="8" t="s">
+      <c r="D13" s="5" t="s">
         <v>98</v>
       </c>
-      <c r="B11" s="6" t="s">
-        <v>78</v>
-      </c>
-      <c r="C11" s="6" t="s">
+    </row>
+    <row r="14" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A14" s="6" t="s">
         <v>99</v>
       </c>
-    </row>
-    <row r="12" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A12" s="8" t="s">
+      <c r="B14" s="5" t="s">
         <v>100</v>
       </c>
-      <c r="B12" s="6" t="s">
-        <v>78</v>
-      </c>
-      <c r="C12" s="6" t="s">
+      <c r="C14" s="5" t="s">
         <v>101</v>
       </c>
     </row>
-    <row r="13" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A13" s="8" t="s">
+    <row r="15" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A15" s="6" t="s">
         <v>102</v>
       </c>
-      <c r="B13" s="6" t="s">
-        <v>78</v>
-      </c>
-      <c r="C13" s="6" t="s">
+      <c r="B15" s="5" t="s">
+        <v>100</v>
+      </c>
+      <c r="C15" s="5" t="s">
         <v>103</v>
       </c>
-      <c r="D13" s="6" t="s">
+    </row>
+    <row r="16" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A16" s="6" t="s">
         <v>104</v>
       </c>
-    </row>
-    <row r="14" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A14" s="8" t="s">
+      <c r="B16" s="5" t="s">
+        <v>72</v>
+      </c>
+      <c r="C16" s="5" t="s">
         <v>105</v>
       </c>
-      <c r="B14" s="6" t="s">
-        <v>78</v>
-      </c>
-      <c r="C14" s="6" t="s">
-        <v>103</v>
-      </c>
-      <c r="D14" s="6" t="s">
+      <c r="D16" s="5" t="s">
         <v>106</v>
       </c>
     </row>
-    <row r="15" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A15" s="8" t="s">
+    <row r="17" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A17" s="6" t="s">
         <v>107</v>
       </c>
-      <c r="B15" s="6" t="s">
-        <v>78</v>
-      </c>
-      <c r="C15" s="6" t="s">
+      <c r="B17" s="5" t="s">
+        <v>72</v>
+      </c>
+      <c r="C17" s="5" t="s">
+        <v>105</v>
+      </c>
+      <c r="D17" s="5" t="s">
         <v>108</v>
       </c>
     </row>
-    <row r="16" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A16" s="8" t="s">
+    <row r="18" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A18" s="6" t="s">
         <v>109</v>
       </c>
-      <c r="B16" s="6" t="s">
-        <v>78</v>
-      </c>
-      <c r="C16" s="6" t="s">
+      <c r="B18" s="5" t="s">
+        <v>72</v>
+      </c>
+      <c r="C18" s="5" t="s">
         <v>110</v>
       </c>
-      <c r="D16" s="6" t="s">
+    </row>
+    <row r="19" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A19" s="6" t="s">
         <v>111</v>
       </c>
-    </row>
-    <row r="17" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A17" s="8" t="s">
-        <v>109</v>
-      </c>
-      <c r="B17" s="6" t="s">
-        <v>78</v>
-      </c>
-      <c r="C17" s="6" t="s">
+      <c r="B19" s="5" t="s">
+        <v>72</v>
+      </c>
+      <c r="C19" s="5" t="s">
         <v>112</v>
       </c>
-      <c r="D17" s="6" t="s">
+      <c r="D19" s="5" t="s">
         <v>113</v>
       </c>
     </row>
-    <row r="18" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A18" s="8" t="s">
-        <v>109</v>
-      </c>
-      <c r="B18" s="6" t="s">
-        <v>78</v>
-      </c>
-      <c r="C18" s="6" t="s">
+    <row r="20" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A20" s="6" t="s">
+        <v>111</v>
+      </c>
+      <c r="B20" s="5" t="s">
+        <v>72</v>
+      </c>
+      <c r="C20" s="5" t="s">
         <v>114</v>
       </c>
-      <c r="D18" s="6" t="s">
+      <c r="D20" s="5" t="s">
         <v>115</v>
       </c>
     </row>
-    <row r="19" customFormat="false" ht="45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A19" s="8" t="s">
+    <row r="21" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A21" s="6" t="s">
+        <v>111</v>
+      </c>
+      <c r="B21" s="5" t="s">
+        <v>72</v>
+      </c>
+      <c r="C21" s="5" t="s">
         <v>116</v>
       </c>
-      <c r="B19" s="7" t="s">
+      <c r="D21" s="5" t="s">
         <v>117</v>
       </c>
-      <c r="C19" s="7" t="s">
+    </row>
+    <row r="22" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A22" s="6" t="s">
         <v>118</v>
       </c>
-      <c r="D19" s="9" t="s">
+      <c r="B22" s="5" t="s">
         <v>119</v>
       </c>
-    </row>
-    <row r="20" customFormat="false" ht="45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A20" s="8" t="s">
+      <c r="C22" s="5" t="s">
         <v>120</v>
       </c>
-      <c r="B20" s="7" t="s">
-        <v>117</v>
-      </c>
-      <c r="C20" s="7" t="s">
+    </row>
+    <row r="23" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A23" s="6" t="s">
         <v>121</v>
       </c>
-      <c r="D20" s="9" t="s">
-        <v>119</v>
-      </c>
-    </row>
-    <row r="21" customFormat="false" ht="45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A21" s="8" t="s">
+      <c r="B23" s="5" t="s">
         <v>122</v>
       </c>
-      <c r="B21" s="7" t="s">
-        <v>117</v>
-      </c>
-      <c r="C21" s="7" t="s">
+      <c r="C23" s="5" t="s">
         <v>123</v>
       </c>
-      <c r="D21" s="9" t="s">
-        <v>119</v>
-      </c>
-    </row>
-    <row r="22" customFormat="false" ht="45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A22" s="8" t="s">
+    </row>
+    <row r="24" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A24" s="6" t="s">
         <v>124</v>
       </c>
-      <c r="B22" s="7" t="s">
-        <v>117</v>
-      </c>
-      <c r="C22" s="7" t="s">
+      <c r="B24" s="5" t="s">
         <v>125</v>
       </c>
-      <c r="D22" s="9" t="s">
+      <c r="C24" s="5" t="s">
         <v>126</v>
       </c>
-    </row>
-    <row r="23" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A23" s="8" t="s">
+      <c r="D24" s="5" t="s">
         <v>127</v>
       </c>
-      <c r="B23" s="6" t="s">
+    </row>
+    <row r="25" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A25" s="6" t="s">
+        <v>124</v>
+      </c>
+      <c r="B25" s="5" t="s">
         <v>128</v>
       </c>
-      <c r="C23" s="6" t="s">
+      <c r="C25" s="5" t="s">
         <v>129</v>
       </c>
-    </row>
-    <row r="24" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A24" s="8" t="s">
+      <c r="D25" s="5" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="26" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A26" s="6" t="s">
         <v>130</v>
       </c>
-      <c r="B24" s="6" t="s">
-        <v>128</v>
-      </c>
-      <c r="C24" s="6" t="s">
+      <c r="B26" s="5" t="s">
+        <v>122</v>
+      </c>
+      <c r="C26" s="5" t="s">
         <v>131</v>
       </c>
-    </row>
-    <row r="25" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A25" s="8" t="s">
+      <c r="D26" s="5" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="27" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A27" s="6" t="s">
         <v>132</v>
       </c>
-      <c r="B25" s="6" t="s">
+      <c r="B27" s="5" t="s">
+        <v>122</v>
+      </c>
+      <c r="C27" s="5" t="s">
         <v>133</v>
       </c>
-      <c r="C25" s="6" t="s">
+      <c r="D27" s="5" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="28" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A28" s="6" t="s">
         <v>134</v>
       </c>
-      <c r="D25" s="6" t="s">
+      <c r="B28" s="5" t="s">
+        <v>122</v>
+      </c>
+      <c r="C28" s="5" t="s">
         <v>135</v>
       </c>
-    </row>
-    <row r="26" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A26" s="8" t="s">
+      <c r="D28" s="5" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="29" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A29" s="6" t="s">
         <v>136</v>
       </c>
-      <c r="B26" s="6" t="s">
+      <c r="B29" s="5" t="s">
+        <v>122</v>
+      </c>
+      <c r="C29" s="5" t="s">
         <v>137</v>
       </c>
-      <c r="C26" s="6" t="s">
+    </row>
+    <row r="30" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A30" s="6" t="s">
         <v>138</v>
       </c>
-    </row>
-    <row r="27" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A27" s="8" t="s">
+      <c r="B30" s="5" t="s">
+        <v>122</v>
+      </c>
+      <c r="C30" s="5" t="s">
         <v>139</v>
       </c>
-      <c r="B27" s="6" t="s">
+    </row>
+    <row r="31" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A31" s="6" t="s">
         <v>140</v>
       </c>
-      <c r="C27" s="6" t="s">
+      <c r="B31" s="5" t="s">
         <v>141</v>
       </c>
-    </row>
-    <row r="28" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A28" s="8" t="s">
+      <c r="C31" s="5" t="s">
         <v>142</v>
       </c>
-      <c r="B28" s="6" t="s">
+    </row>
+    <row r="32" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A32" s="7" t="s">
         <v>143</v>
       </c>
-      <c r="C28" s="6" t="s">
+      <c r="B32" s="7" t="s">
         <v>144</v>
       </c>
-      <c r="D28" s="6" t="s">
+      <c r="C32" s="7" t="s">
         <v>145</v>
       </c>
-    </row>
-    <row r="29" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A29" s="8" t="s">
-        <v>142</v>
-      </c>
-      <c r="B29" s="6" t="s">
+      <c r="D32" s="7" t="s">
         <v>146</v>
-      </c>
-      <c r="C29" s="6" t="s">
-        <v>147</v>
-      </c>
-      <c r="D29" s="6" t="s">
-        <v>145</v>
-      </c>
-    </row>
-    <row r="30" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A30" s="8" t="s">
-        <v>148</v>
-      </c>
-      <c r="B30" s="6" t="s">
-        <v>140</v>
-      </c>
-      <c r="C30" s="6" t="s">
-        <v>149</v>
-      </c>
-      <c r="D30" s="6" t="s">
-        <v>145</v>
-      </c>
-    </row>
-    <row r="31" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A31" s="8" t="s">
-        <v>150</v>
-      </c>
-      <c r="B31" s="6" t="s">
-        <v>140</v>
-      </c>
-      <c r="C31" s="6" t="s">
-        <v>151</v>
-      </c>
-      <c r="D31" s="6" t="s">
-        <v>145</v>
-      </c>
-    </row>
-    <row r="32" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A32" s="8" t="s">
-        <v>152</v>
-      </c>
-      <c r="B32" s="6" t="s">
-        <v>140</v>
-      </c>
-      <c r="C32" s="6" t="s">
-        <v>153</v>
-      </c>
-      <c r="D32" s="6" t="s">
-        <v>145</v>
-      </c>
-    </row>
-    <row r="33" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A33" s="8" t="s">
-        <v>154</v>
-      </c>
-      <c r="B33" s="6" t="s">
-        <v>140</v>
-      </c>
-      <c r="C33" s="6" t="s">
-        <v>155</v>
-      </c>
-    </row>
-    <row r="34" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A34" s="8" t="s">
-        <v>156</v>
-      </c>
-      <c r="B34" s="6" t="s">
-        <v>140</v>
-      </c>
-      <c r="C34" s="6" t="s">
-        <v>157</v>
-      </c>
-    </row>
-    <row r="35" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A35" s="8" t="s">
-        <v>158</v>
-      </c>
-      <c r="B35" s="6" t="s">
-        <v>159</v>
-      </c>
-      <c r="C35" s="6" t="s">
-        <v>160</v>
-      </c>
-    </row>
-    <row r="36" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A36" s="7" t="s">
-        <v>161</v>
-      </c>
-      <c r="B36" s="7" t="s">
-        <v>162</v>
-      </c>
-      <c r="C36" s="7" t="s">
-        <v>163</v>
-      </c>
-      <c r="D36" s="7" t="s">
-        <v>164</v>
       </c>
     </row>
   </sheetData>
@@ -1667,8 +1476,8 @@
   </sheetPr>
   <dimension ref="A1:C21"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A2" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B16" activeCellId="0" sqref="B16"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A2" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A3" activeCellId="0" sqref="A3:A21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.578125" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1680,7 +1489,7 @@
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="0" t="s">
-        <v>165</v>
+        <v>147</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1688,219 +1497,219 @@
         <v>1</v>
       </c>
       <c r="B2" s="1" t="s">
+        <v>148</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="8" t="s">
+        <v>132</v>
+      </c>
+      <c r="B3" s="6" t="s">
+        <v>149</v>
+      </c>
+      <c r="C3" s="9" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="8" t="s">
+        <v>151</v>
+      </c>
+      <c r="B4" s="6" t="s">
+        <v>149</v>
+      </c>
+      <c r="C4" s="9" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="8" t="s">
+        <v>134</v>
+      </c>
+      <c r="B5" s="6" t="s">
+        <v>149</v>
+      </c>
+      <c r="C5" s="9" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="8" t="s">
+        <v>154</v>
+      </c>
+      <c r="B6" s="6" t="s">
+        <v>155</v>
+      </c>
+      <c r="C6" s="9" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="8" t="s">
+        <v>118</v>
+      </c>
+      <c r="B7" s="6" t="s">
+        <v>155</v>
+      </c>
+      <c r="C7" s="9" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A8" s="8" t="s">
+        <v>158</v>
+      </c>
+      <c r="B8" s="6" t="s">
+        <v>155</v>
+      </c>
+      <c r="C8" s="9" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A9" s="8" t="s">
+        <v>160</v>
+      </c>
+      <c r="B9" s="6" t="s">
+        <v>161</v>
+      </c>
+      <c r="C9" s="9" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A10" s="8" t="s">
+        <v>163</v>
+      </c>
+      <c r="B10" s="6" t="s">
+        <v>161</v>
+      </c>
+      <c r="C10" s="9" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A11" s="8" t="s">
+        <v>165</v>
+      </c>
+      <c r="B11" s="6" t="s">
+        <v>161</v>
+      </c>
+      <c r="C11" s="9" t="s">
         <v>166</v>
       </c>
-      <c r="C2" s="1" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="10" t="s">
-        <v>150</v>
-      </c>
-      <c r="B3" s="8" t="s">
+    </row>
+    <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A12" s="8" t="s">
         <v>167</v>
       </c>
-      <c r="C3" s="11" t="s">
+      <c r="B12" s="6" t="s">
         <v>168</v>
       </c>
-    </row>
-    <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="10" t="s">
+      <c r="C12" s="9" t="s">
         <v>169</v>
       </c>
-      <c r="B4" s="8" t="s">
-        <v>167</v>
-      </c>
-      <c r="C4" s="11" t="s">
+    </row>
+    <row r="13" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A13" s="8" t="s">
         <v>170</v>
       </c>
-    </row>
-    <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="10" t="s">
-        <v>152</v>
-      </c>
-      <c r="B5" s="8" t="s">
-        <v>167</v>
-      </c>
-      <c r="C5" s="11" t="s">
+      <c r="B13" s="6" t="s">
+        <v>168</v>
+      </c>
+      <c r="C13" s="9" t="s">
         <v>171</v>
       </c>
     </row>
-    <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="10" t="s">
+    <row r="14" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A14" s="8" t="s">
         <v>172</v>
       </c>
-      <c r="B6" s="8" t="s">
+      <c r="B14" s="6" t="s">
+        <v>168</v>
+      </c>
+      <c r="C14" s="9" t="s">
         <v>173</v>
       </c>
-      <c r="C6" s="11" t="s">
+    </row>
+    <row r="15" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A15" s="8" t="s">
         <v>174</v>
       </c>
-    </row>
-    <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="10" t="s">
-        <v>136</v>
-      </c>
-      <c r="B7" s="8" t="s">
-        <v>173</v>
-      </c>
-      <c r="C7" s="11" t="s">
+      <c r="B15" s="6" t="s">
+        <v>168</v>
+      </c>
+      <c r="C15" s="9" t="s">
         <v>175</v>
       </c>
     </row>
-    <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="10" t="s">
+    <row r="16" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A16" s="8" t="s">
         <v>176</v>
       </c>
-      <c r="B8" s="8" t="s">
-        <v>173</v>
-      </c>
-      <c r="C8" s="11" t="s">
+      <c r="B16" s="6" t="s">
+        <v>168</v>
+      </c>
+      <c r="C16" s="9" t="s">
         <v>177</v>
       </c>
     </row>
-    <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="10" t="s">
+    <row r="17" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A17" s="8" t="s">
         <v>178</v>
       </c>
-      <c r="B9" s="8" t="s">
+      <c r="B17" s="6" t="s">
         <v>179</v>
       </c>
-      <c r="C9" s="11" t="s">
+      <c r="C17" s="9" t="s">
         <v>180</v>
       </c>
     </row>
-    <row r="10" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="10" t="s">
+    <row r="18" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A18" s="8" t="s">
         <v>181</v>
       </c>
-      <c r="B10" s="8" t="s">
+      <c r="B18" s="6" t="s">
         <v>179</v>
       </c>
-      <c r="C10" s="11" t="s">
+      <c r="C18" s="9" t="s">
         <v>182</v>
       </c>
     </row>
-    <row r="11" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="10" t="s">
+    <row r="19" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A19" s="8" t="s">
+        <v>121</v>
+      </c>
+      <c r="B19" s="6" t="s">
         <v>183</v>
       </c>
-      <c r="B11" s="8" t="s">
-        <v>179</v>
-      </c>
-      <c r="C11" s="11" t="s">
+      <c r="C19" s="9" t="s">
         <v>184</v>
       </c>
     </row>
-    <row r="12" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A12" s="10" t="s">
+    <row r="20" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A20" s="8" t="s">
         <v>185</v>
       </c>
-      <c r="B12" s="8" t="s">
+      <c r="B20" s="6" t="s">
+        <v>183</v>
+      </c>
+      <c r="C20" s="9" t="s">
         <v>186</v>
       </c>
-      <c r="C12" s="11" t="s">
+    </row>
+    <row r="21" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A21" s="8" t="s">
         <v>187</v>
       </c>
-    </row>
-    <row r="13" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A13" s="10" t="s">
+      <c r="B21" s="6" t="s">
         <v>188</v>
       </c>
-      <c r="B13" s="8" t="s">
-        <v>186</v>
-      </c>
-      <c r="C13" s="11" t="s">
+      <c r="C21" s="9" t="s">
         <v>189</v>
-      </c>
-    </row>
-    <row r="14" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A14" s="10" t="s">
-        <v>190</v>
-      </c>
-      <c r="B14" s="8" t="s">
-        <v>186</v>
-      </c>
-      <c r="C14" s="11" t="s">
-        <v>191</v>
-      </c>
-    </row>
-    <row r="15" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A15" s="10" t="s">
-        <v>192</v>
-      </c>
-      <c r="B15" s="8" t="s">
-        <v>186</v>
-      </c>
-      <c r="C15" s="11" t="s">
-        <v>193</v>
-      </c>
-    </row>
-    <row r="16" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A16" s="10" t="s">
-        <v>194</v>
-      </c>
-      <c r="B16" s="8" t="s">
-        <v>186</v>
-      </c>
-      <c r="C16" s="11" t="s">
-        <v>195</v>
-      </c>
-    </row>
-    <row r="17" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A17" s="10" t="s">
-        <v>196</v>
-      </c>
-      <c r="B17" s="8" t="s">
-        <v>197</v>
-      </c>
-      <c r="C17" s="11" t="s">
-        <v>198</v>
-      </c>
-    </row>
-    <row r="18" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A18" s="10" t="s">
-        <v>199</v>
-      </c>
-      <c r="B18" s="8" t="s">
-        <v>197</v>
-      </c>
-      <c r="C18" s="11" t="s">
-        <v>200</v>
-      </c>
-    </row>
-    <row r="19" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A19" s="10" t="s">
-        <v>139</v>
-      </c>
-      <c r="B19" s="8" t="s">
-        <v>201</v>
-      </c>
-      <c r="C19" s="11" t="s">
-        <v>202</v>
-      </c>
-    </row>
-    <row r="20" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A20" s="10" t="s">
-        <v>203</v>
-      </c>
-      <c r="B20" s="8" t="s">
-        <v>201</v>
-      </c>
-      <c r="C20" s="11" t="s">
-        <v>204</v>
-      </c>
-    </row>
-    <row r="21" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A21" s="10" t="s">
-        <v>205</v>
-      </c>
-      <c r="B21" s="8" t="s">
-        <v>206</v>
-      </c>
-      <c r="C21" s="11" t="s">
-        <v>207</v>
       </c>
     </row>
   </sheetData>

</xml_diff>